<commit_message>
Updating loggers & tags
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>source</t>
   </si>
@@ -25,13 +25,43 @@
     <t>children</t>
   </si>
   <si>
-    <t>BLR</t>
-  </si>
-  <si>
-    <t>LONDON</t>
-  </si>
-  <si>
-    <t>DEL</t>
+    <t>child_age</t>
+  </si>
+  <si>
+    <t>round_trip</t>
+  </si>
+  <si>
+    <t>direct_flights</t>
+  </si>
+  <si>
+    <t>cabin_class</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Shenzhen</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Bhopal</t>
+  </si>
+  <si>
+    <t>Premium economy</t>
   </si>
 </sst>
 </file>
@@ -58,15 +88,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -76,16 +112,103 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -95,17 +218,56 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -125,6 +287,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -276,9 +439,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -358,7 +521,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -385,10 +548,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -635,9 +798,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -915,7 +1078,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -942,10 +1105,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1187,14 +1350,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="8.85156" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="8" width="18.0078" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1210,34 +1374,156 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
+      <c r="F2" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s" s="9">
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6">
         <v>5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>1</v>
       </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>